<commit_message>
Excel management moved to ExcelManager and removed from CLIMenu, png and jpg added to FileHandle
</commit_message>
<xml_diff>
--- a/Source/DCMT_Results.xlsx
+++ b/Source/DCMT_Results.xlsx
@@ -378,12 +378,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Planes</t>
+          <t>Planes.pdf</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>docx</t>
+          <t>pdf</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -420,12 +420,12 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Trains</t>
+          <t>Trains.jpg</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>pdf</t>
+          <t>jpg</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -462,12 +462,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Automobiles</t>
+          <t>Automobiles.docx</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>jpeg</t>
+          <t>docx</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">

</xml_diff>

<commit_message>
More functions added to ExcelManager
</commit_message>
<xml_diff>
--- a/Source/DCMT_Results.xlsx
+++ b/Source/DCMT_Results.xlsx
@@ -366,12 +366,32 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
+          <t>Bucket Location</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
           <t>File Tag 1</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>File Tag 2</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>File Tag 3</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>File Tag 4</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>File Tag 5</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
ExcelManager, keyword selection implemented and adding an entry
</commit_message>
<xml_diff>
--- a/Source/DCMT_Results.xlsx
+++ b/Source/DCMT_Results.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -356,91 +356,71 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>File Name</t>
+          <t>FILE_NAME</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>File Type</t>
+          <t>FILE_TYPE</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Bucket Location</t>
+          <t>BUCKET_LOCATION</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>File Tag 1</t>
+          <t>FILE_TAG_1</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>File Tag 2</t>
+          <t>FILE_TAG_2</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>File Tag 3</t>
+          <t>FILE_TAG_3</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>File Tag 4</t>
+          <t>FILE_TAG_4</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>File Tag 5</t>
+          <t>FILE_TAG_5</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Planes.pdf</t>
+          <t>AWS-Achieves_FED-Ramp-JPEG-2.jpg</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>pdf</t>
+          <t>jpg</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>aviation</t>
+          <t>uconn-sdp-team11-unprocessed-docs</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>documentation</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>locomotive</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>promotional</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>automotive</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>image</t>
+          <t>the</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Trains.jpg</t>
+          <t>AWS-Achieves_FED-Ramp-JPEG.jpg</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -450,74 +430,27 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>aviation</t>
+          <t>uconn-sdp-team11-unprocessed-docs</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>documentation</t>
+          <t>a</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>locomotive</t>
+          <t>for</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>promotional</t>
+          <t>is</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>automotive</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>image</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Automobiles.docx</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>docx</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>aviation</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>documentation</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>locomotive</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>promotional</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>automotive</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>image</t>
+          <t>the</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Added AWS tagging (TagFile function implementation).
</commit_message>
<xml_diff>
--- a/Source/DCMT_Results.xlsx
+++ b/Source/DCMT_Results.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -454,6 +454,102 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Test3PagePDF_Seven_Ways_to_Apply_the_Cyber_Kill_Chain_with_a_Threat_Intelligence_Platform-page-003.pdf</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>pdf</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>uconn-sdp-team11-unprocessed-docs</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>and</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>cyber</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>the</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Test3PagePDF_Seven_Ways_to_Apply_the_Cyber_Kill_Chain_with_a_Threat_Intelligence_Platform-page-003.pdf</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>pdf</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>uconn-sdp-team11-unprocessed-docs</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>and</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>cyber</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>the</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Test3PagePDF_Seven_Ways_to_Apply_the_Cyber_Kill_Chain_with_a_Threat_Intelligence_Platform-page-003.pdf</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>pdf</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>uconn-sdp-team11-unprocessed-docs</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>and</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>cyber</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>the</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Stitched together the moving, tagging, and deletion functions.
</commit_message>
<xml_diff>
--- a/Source/DCMT_Results.xlsx
+++ b/Source/DCMT_Results.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -467,7 +467,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>uconn-sdp-team11-unprocessed-docs</t>
+          <t>uconn-sdp-team11-tagged-docs</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -547,6 +547,119 @@
       <c r="F6" t="inlineStr">
         <is>
           <t>the</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Test3PagePDF_Seven_Ways_to_Apply_the_Cyber_Kill_Chain_with_a_Threat_Intelligence_Platform-page-003.pdf</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>pdf</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>uconn-sdp-team11-unprocessed-docs</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>and</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>cyber</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>the</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Test3PagePDF_Seven_Ways_to_Apply_the_Cyber_Kill_Chain_with_a_Threat_Intelligence_Platform-page-003.pdf</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>pdf</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>uconn-sdp-team11-unprocessed-docs</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>cyber</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>threat</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>catch-can-detecting-server-side-request-forgery-attacks-amazon-web-services_13843.pdf</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>pdf</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>uconn-sdp-team11-tagged-docs</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>attack</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>catch-can-detecting-server-side-request-forgery-attacks-amazon-web-services_13843.pdf</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>pdf</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>uconn-sdp-team11-unprocessed-docs</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>attacks</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>detection</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>request</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Commented out redundant print statements.
</commit_message>
<xml_diff>
--- a/Source/DCMT_Results.xlsx
+++ b/Source/DCMT_Results.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -663,6 +663,38 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>LM-White-Paper-Threat-Driven-Approach.pdf</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>pdf</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>uconn-sdp-team11-tagged-docs</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>defense</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>lm</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>threat</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>